<commit_message>
cals have alarms now
</commit_message>
<xml_diff>
--- a/content/about/Schedule.xlsx
+++ b/content/about/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DonsLaptop\Desktop\GitHub\ledatascifi-2025\content\about\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280F03E8-CD98-4231-8B85-AB027D1FD0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9772EB62-F405-4BFB-85E0-D31750165BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{C4EC7618-C1C5-4BB6-84C2-5B870F390279}"/>
   </bookViews>
@@ -719,7 +719,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -848,6 +848,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1523,7 +1524,7 @@
   <dimension ref="A1:R226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1836,7 +1837,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1853,7 +1854,7 @@
       <c r="F13" s="13">
         <v>45313</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H13" s="17" t="s">
@@ -1880,7 +1881,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1897,7 +1898,7 @@
       <c r="F14" s="13">
         <v>45313</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="44" t="s">
         <v>20</v>
       </c>
       <c r="H14" s="17" t="s">
@@ -1926,7 +1927,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="87" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1943,7 +1944,7 @@
       <c r="F15" s="13">
         <v>45313</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="44" t="s">
         <v>22</v>
       </c>
       <c r="H15" s="17" t="s">
@@ -1972,7 +1973,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14.1</v>
       </c>
@@ -1989,7 +1990,7 @@
       <c r="F16" s="13">
         <v>45314</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="44" t="s">
         <v>23</v>
       </c>
       <c r="H16" s="17" t="s">
@@ -2161,7 +2162,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -2178,7 +2179,7 @@
       <c r="F21" s="19">
         <v>45315</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="44" t="s">
         <v>26</v>
       </c>
       <c r="H21" s="17" t="s">
@@ -2249,7 +2250,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>17.2</v>
       </c>
@@ -2266,7 +2267,7 @@
       <c r="F23" s="19">
         <v>45315</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="44" t="s">
         <v>29</v>
       </c>
       <c r="H23" s="17" t="s">
@@ -2547,7 +2548,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>26.5</v>
       </c>
@@ -2564,7 +2565,7 @@
       <c r="F31" s="19">
         <v>45320</v>
       </c>
-      <c r="G31" s="17" t="s">
+      <c r="G31" s="44" t="s">
         <v>35</v>
       </c>
       <c r="H31" s="17" t="s">
@@ -2635,7 +2636,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>27.1</v>
       </c>
@@ -2652,7 +2653,7 @@
       <c r="F33" s="19">
         <v>45320</v>
       </c>
-      <c r="G33" s="17" t="s">
+      <c r="G33" s="44" t="s">
         <v>37</v>
       </c>
       <c r="H33" s="17" t="s">
@@ -2758,7 +2759,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" ht="174" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>31</v>
       </c>
@@ -2775,7 +2776,7 @@
       <c r="F36" s="19">
         <v>45322</v>
       </c>
-      <c r="G36" s="17" t="s">
+      <c r="G36" s="44" t="s">
         <v>39</v>
       </c>
       <c r="H36" s="17" t="s">
@@ -3880,7 +3881,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>62</v>
       </c>
@@ -3897,7 +3898,7 @@
       <c r="F66" s="13">
         <v>45329</v>
       </c>
-      <c r="G66" s="17" t="s">
+      <c r="G66" s="44" t="s">
         <v>62</v>
       </c>
       <c r="H66" s="17" t="s">
@@ -6690,7 +6691,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -9543,20 +9544,10 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G21" r:id="rId1" xr:uid="{BB099E47-7FF5-41CE-AAF7-A77A8CFF3913}"/>
-    <hyperlink ref="G13" r:id="rId2" xr:uid="{3AA9989C-9EEB-4718-A411-408DFFE8A965}"/>
-    <hyperlink ref="G14" r:id="rId3" xr:uid="{1874924A-1AE9-41C0-9173-3489A9096F49}"/>
-    <hyperlink ref="G36" r:id="rId4" display="Chapter 2 (basic syntax) to 14 (modules)" xr:uid="{3255AB21-7541-4BF2-83F3-3E94C5712664}"/>
-    <hyperlink ref="G66" r:id="rId5" xr:uid="{6931D715-50E7-411F-909D-5849DD40C628}"/>
-    <hyperlink ref="G31" r:id="rId6" xr:uid="{4A294440-1502-4A36-9E24-43501A9B4B04}"/>
-    <hyperlink ref="G23" r:id="rId7" xr:uid="{3A343C54-588F-4EE4-A684-BEAC7E066F79}"/>
-    <hyperlink ref="G33" r:id="rId8" xr:uid="{74E0F602-4AD5-4DB2-94D9-EE31C0B1A8CC}"/>
-    <hyperlink ref="G112" r:id="rId9" xr:uid="{C8D7C107-7C07-41CA-A2CD-31DDAFF3FDF8}"/>
-    <hyperlink ref="G16" r:id="rId10" display="Once I accept you into the organization, go to the GitHub discussion board and:" xr:uid="{581D3263-F357-4CC0-8037-85ECE40E0165}"/>
-    <hyperlink ref="E141" r:id="rId11" xr:uid="{07E3D8FE-19F7-46BC-B625-DD8BCFA50F3C}"/>
-    <hyperlink ref="G15" r:id="rId12" xr:uid="{FACE2ED2-97E0-440E-8529-7CC59DFCE43C}"/>
+    <hyperlink ref="G112" r:id="rId1" xr:uid="{C8D7C107-7C07-41CA-A2CD-31DDAFF3FDF8}"/>
+    <hyperlink ref="E141" r:id="rId2" xr:uid="{07E3D8FE-19F7-46BC-B625-DD8BCFA50F3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
schedule for 2025 ready
</commit_message>
<xml_diff>
--- a/content/about/Schedule.xlsx
+++ b/content/about/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DonsLaptop\Desktop\GitHub\ledatascifi-2025\content\about\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77187AA-0D31-48FA-A86A-AA6DA47D5A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2825D628-7233-44AD-971C-F76C94886FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{C4EC7618-C1C5-4BB6-84C2-5B870F390279}"/>
   </bookViews>
@@ -1572,7 +1572,7 @@
   <dimension ref="A1:L208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>